<commit_message>
got the required excel file
</commit_message>
<xml_diff>
--- a/JAN-22/CNH/FAS 42 HP JAN-22.xlsx
+++ b/JAN-22/CNH/FAS 42 HP JAN-22.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\Excel_automation-master\JAN-22\CNH\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="12120" windowHeight="4800"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'42 HP'!$A$4:$AI$55</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -803,12 +808,51 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,45 +864,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,6 +874,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1032,11 +1040,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="135318144"/>
-        <c:axId val="138052352"/>
+        <c:axId val="1048258352"/>
+        <c:axId val="999297664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135318144"/>
+        <c:axId val="1048258352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="138052352"/>
+        <c:crossAx val="999297664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1120,7 +1128,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138052352"/>
+        <c:axId val="999297664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1202,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135318144"/>
+        <c:crossAx val="1048258352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1325,7 +1333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1360,7 +1368,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1604,117 +1612,117 @@
     <row r="1" spans="1:59" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:59" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="64"/>
-      <c r="AI2" s="65"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="57"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="58"/>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
-      <c r="W3" s="66"/>
-      <c r="X3" s="66"/>
-      <c r="Y3" s="66"/>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66"/>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="66"/>
-      <c r="AF3" s="66"/>
-      <c r="AG3" s="66"/>
-      <c r="AH3" s="66"/>
-      <c r="AI3" s="67"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="60"/>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="72"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="72"/>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="72"/>
-      <c r="AG4" s="72"/>
-      <c r="AH4" s="72"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:59" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1765,13 +1773,13 @@
       </c>
     </row>
     <row r="6" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="74"/>
+      <c r="B6" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="68"/>
       <c r="D6" s="12">
         <v>1</v>
       </c>
@@ -1868,7 +1876,7 @@
       <c r="AI6" s="11"/>
     </row>
     <row r="7" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
@@ -1914,7 +1922,7 @@
       </c>
     </row>
     <row r="8" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="15" t="s">
         <v>22</v>
       </c>
@@ -1959,7 +1967,7 @@
       </c>
     </row>
     <row r="9" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="15" t="s">
         <v>2</v>
       </c>
@@ -2070,7 +2078,7 @@
       </c>
     </row>
     <row r="10" spans="1:59" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="21" t="s">
         <v>14</v>
       </c>
@@ -2205,10 +2213,10 @@
       </c>
     </row>
     <row r="11" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="69" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="12"/>
@@ -2273,8 +2281,8 @@
       <c r="BG11" s="29"/>
     </row>
     <row r="12" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="63"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="13" t="s">
         <v>15</v>
       </c>
@@ -2432,8 +2440,8 @@
       <c r="BG12" s="29"/>
     </row>
     <row r="13" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="63" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="70" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="13"/>
@@ -2474,8 +2482,8 @@
       </c>
     </row>
     <row r="14" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="63"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="13" t="s">
         <v>15</v>
       </c>
@@ -2609,8 +2617,8 @@
       </c>
     </row>
     <row r="15" spans="1:59" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="63" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="13"/>
@@ -2651,8 +2659,8 @@
       </c>
     </row>
     <row r="16" spans="1:59" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="63"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="32" t="s">
         <v>15</v>
       </c>
@@ -2786,8 +2794,8 @@
       </c>
     </row>
     <row r="17" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="63" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="70" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="13"/>
@@ -2828,8 +2836,8 @@
       </c>
     </row>
     <row r="18" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="63"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="32" t="s">
         <v>15</v>
       </c>
@@ -2963,8 +2971,8 @@
       </c>
     </row>
     <row r="19" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="63" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="70" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="13"/>
@@ -3009,8 +3017,8 @@
       </c>
     </row>
     <row r="20" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="32" t="s">
         <v>15</v>
       </c>
@@ -3144,8 +3152,8 @@
       </c>
     </row>
     <row r="21" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="63" t="s">
+      <c r="A21" s="61"/>
+      <c r="B21" s="70" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="13"/>
@@ -3186,8 +3194,8 @@
       </c>
     </row>
     <row r="22" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="32" t="s">
         <v>15</v>
       </c>
@@ -3321,8 +3329,8 @@
       </c>
     </row>
     <row r="23" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="58"/>
-      <c r="B23" s="63" t="s">
+      <c r="A23" s="61"/>
+      <c r="B23" s="70" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="13"/>
@@ -3363,8 +3371,8 @@
       </c>
     </row>
     <row r="24" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
-      <c r="B24" s="63"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="32" t="s">
         <v>15</v>
       </c>
@@ -3498,8 +3506,8 @@
       </c>
     </row>
     <row r="25" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
-      <c r="B25" s="63" t="s">
+      <c r="A25" s="61"/>
+      <c r="B25" s="70" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="13"/>
@@ -3542,8 +3550,8 @@
       </c>
     </row>
     <row r="26" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="70"/>
       <c r="C26" s="32" t="s">
         <v>15</v>
       </c>
@@ -3677,8 +3685,8 @@
       </c>
     </row>
     <row r="27" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="58"/>
-      <c r="B27" s="59" t="s">
+      <c r="A27" s="61"/>
+      <c r="B27" s="72" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="13"/>
@@ -3719,8 +3727,8 @@
       </c>
     </row>
     <row r="28" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
-      <c r="B28" s="60"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="32" t="s">
         <v>15</v>
       </c>
@@ -3854,8 +3862,8 @@
       </c>
     </row>
     <row r="29" spans="1:35" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="58"/>
-      <c r="B29" s="61" t="s">
+      <c r="A29" s="61"/>
+      <c r="B29" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="13"/>
@@ -3896,8 +3904,8 @@
       </c>
     </row>
     <row r="30" spans="1:35" s="34" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="58"/>
-      <c r="B30" s="62"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="23" t="s">
         <v>15</v>
       </c>
@@ -4070,7 +4078,7 @@
       <c r="AI31" s="40"/>
     </row>
     <row r="32" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="41"/>
@@ -4109,7 +4117,7 @@
       <c r="AI32" s="42"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="58"/>
+      <c r="A33" s="61"/>
       <c r="B33" s="41"/>
       <c r="C33" s="10"/>
       <c r="D33" s="29"/>
@@ -4146,7 +4154,7 @@
       <c r="AI33" s="42"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="58"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="41"/>
       <c r="C34" s="10"/>
       <c r="D34" s="29"/>
@@ -4183,7 +4191,7 @@
       <c r="AI34" s="42"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="58"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="41"/>
       <c r="C35" s="10"/>
       <c r="D35" s="29"/>
@@ -4220,7 +4228,7 @@
       <c r="AI35" s="42"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="58"/>
+      <c r="A36" s="61"/>
       <c r="B36" s="41"/>
       <c r="C36" s="10"/>
       <c r="D36" s="29"/>
@@ -4257,7 +4265,7 @@
       <c r="AI36" s="42"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
+      <c r="A37" s="61"/>
       <c r="B37" s="41"/>
       <c r="C37" s="10"/>
       <c r="D37" s="29"/>
@@ -4294,7 +4302,7 @@
       <c r="AI37" s="42"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="41"/>
       <c r="C38" s="10"/>
       <c r="D38" s="29"/>
@@ -4331,7 +4339,7 @@
       <c r="AI38" s="42"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="58"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="41"/>
       <c r="C39" s="10"/>
       <c r="D39" s="29"/>
@@ -4368,7 +4376,7 @@
       <c r="AI39" s="42"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="58"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="41"/>
       <c r="C40" s="10"/>
       <c r="D40" s="29"/>
@@ -4405,7 +4413,7 @@
       <c r="AI40" s="42"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="41"/>
       <c r="C41" s="10"/>
       <c r="D41" s="29"/>
@@ -4442,7 +4450,7 @@
       <c r="AI41" s="42"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="58"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="41"/>
       <c r="C42" s="10"/>
       <c r="D42" s="29"/>
@@ -4479,7 +4487,7 @@
       <c r="AI42" s="42"/>
     </row>
     <row r="43" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="58"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="43"/>
       <c r="C43" s="44"/>
       <c r="D43" s="45"/>
@@ -4516,7 +4524,7 @@
       <c r="AI43" s="46"/>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A44" s="58"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="43"/>
       <c r="C44" s="44"/>
       <c r="D44" s="45"/>
@@ -4553,7 +4561,7 @@
       <c r="AI44" s="46"/>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A45" s="58"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="43"/>
       <c r="C45" s="44"/>
       <c r="D45" s="45"/>
@@ -4590,7 +4598,7 @@
       <c r="AI45" s="46"/>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A46" s="58"/>
+      <c r="A46" s="61"/>
       <c r="B46" s="43"/>
       <c r="C46" s="44"/>
       <c r="D46" s="45"/>
@@ -4627,7 +4635,7 @@
       <c r="AI46" s="46"/>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A47" s="58"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="43"/>
       <c r="C47" s="44"/>
       <c r="D47" s="45"/>
@@ -4664,7 +4672,7 @@
       <c r="AI47" s="46"/>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A48" s="58"/>
+      <c r="A48" s="61"/>
       <c r="B48" s="43"/>
       <c r="C48" s="44"/>
       <c r="D48" s="45"/>
@@ -4701,7 +4709,7 @@
       <c r="AI48" s="46"/>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A49" s="58"/>
+      <c r="A49" s="61"/>
       <c r="B49" s="43"/>
       <c r="C49" s="44"/>
       <c r="D49" s="45"/>
@@ -4738,7 +4746,7 @@
       <c r="AI49" s="46"/>
     </row>
     <row r="50" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="68"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="43"/>
       <c r="C50" s="44"/>
       <c r="D50" s="45"/>
@@ -4775,7 +4783,7 @@
       <c r="AI50" s="46"/>
     </row>
     <row r="51" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="63" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="47"/>
@@ -4814,7 +4822,7 @@
       <c r="AI51" s="50"/>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A52" s="70"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="41"/>
       <c r="C52" s="10"/>
       <c r="D52" s="29"/>
@@ -4851,7 +4859,7 @@
       <c r="AI52" s="42"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A53" s="70"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="41"/>
       <c r="C53" s="10"/>
       <c r="D53" s="29"/>
@@ -4888,7 +4896,7 @@
       <c r="AI53" s="42"/>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A54" s="70"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="41"/>
       <c r="C54" s="10"/>
       <c r="D54" s="29"/>
@@ -4925,7 +4933,7 @@
       <c r="AI54" s="42"/>
     </row>
     <row r="55" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="71"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="51"/>
       <c r="C55" s="52"/>
       <c r="D55" s="53"/>
@@ -4964,6 +4972,7 @@
     <row r="56" spans="1:35" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B2:AI3"/>
     <mergeCell ref="A32:A50"/>
     <mergeCell ref="A51:A55"/>
@@ -4980,7 +4989,6 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>